<commit_message>
Version 2.1.1 All function well and compile script added
</commit_message>
<xml_diff>
--- a/jira_input_sample.xlsx
+++ b/jira_input_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtcelec2\Desktop\kaiheng\JIRA_auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22761C1-F1BA-4791-84E3-65C3F6FED9BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C876FF7-975E-4D6C-9CBD-FE83C56C11F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16284" yWindow="-2724" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>DeviceID</t>
   </si>
@@ -93,6 +93,9 @@
   <si>
     <t xml:space="preserve">	
 22627</t>
+  </si>
+  <si>
+    <t>fdafa</t>
   </si>
 </sst>
 </file>
@@ -232,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,10 +296,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,10 +518,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -703,7 +705,9 @@
       <c r="C9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -711,12 +715,11 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
@@ -725,17 +728,31 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="24"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="24"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="24"/>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A10:F10"/>
-  </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{9661DEBF-4E0A-4DF7-93DE-51AD8EAB5DF9}"/>

</xml_diff>